<commit_message>
Added Percentage and rank
</commit_message>
<xml_diff>
--- a/LKG/Result.xlsx
+++ b/LKG/Result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="56">
   <si>
     <t>Student Name</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Total Marks</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Rank</t>
   </si>
   <si>
     <t>Abhik Upadhya</t>
@@ -533,13 +539,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK13"/>
+  <dimension ref="A1:AM13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,16 +657,22 @@
       <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:39">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D2">
         <v>18</v>
@@ -738,42 +750,48 @@
         <v>7.2</v>
       </c>
       <c r="AC2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AD2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AF2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AG2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AI2">
         <v>44.40000000000001</v>
       </c>
       <c r="AJ2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AK2">
         <v>600</v>
       </c>
+      <c r="AL2">
+        <v>7.400000000000001</v>
+      </c>
+      <c r="AM2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:39">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -851,42 +869,48 @@
         <v>24.8</v>
       </c>
       <c r="AC3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AD3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AF3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AI3">
         <v>133.2</v>
       </c>
       <c r="AJ3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AK3">
         <v>600</v>
       </c>
+      <c r="AL3">
+        <v>22.2</v>
+      </c>
+      <c r="AM3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:39">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -964,42 +988,48 @@
         <v>42.8</v>
       </c>
       <c r="AC4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AD4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AI4">
         <v>244.8</v>
       </c>
       <c r="AJ4" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AK4">
         <v>600</v>
       </c>
+      <c r="AL4">
+        <v>40.8</v>
+      </c>
+      <c r="AM4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:39">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1077,42 +1107,48 @@
         <v>34.8</v>
       </c>
       <c r="AC5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AD5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AG5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AI5">
         <v>177.6</v>
       </c>
       <c r="AJ5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AK5">
         <v>600</v>
       </c>
+      <c r="AL5">
+        <v>29.6</v>
+      </c>
+      <c r="AM5">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:39">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1190,42 +1226,48 @@
         <v>15.2</v>
       </c>
       <c r="AC6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AD6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AF6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AG6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AI6">
         <v>118.8</v>
       </c>
       <c r="AJ6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AK6">
         <v>600</v>
       </c>
+      <c r="AL6">
+        <v>19.8</v>
+      </c>
+      <c r="AM6">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:39">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -1303,42 +1345,48 @@
         <v>33.6</v>
       </c>
       <c r="AC7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AD7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AI7">
         <v>214.8</v>
       </c>
       <c r="AJ7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AK7">
         <v>600</v>
       </c>
+      <c r="AL7">
+        <v>35.8</v>
+      </c>
+      <c r="AM7">
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:39">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -1416,42 +1464,48 @@
         <v>45.2</v>
       </c>
       <c r="AC8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AD8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AE8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AH8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AI8">
         <v>265.6</v>
       </c>
       <c r="AJ8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AK8">
         <v>600</v>
       </c>
+      <c r="AL8">
+        <v>44.26666666666667</v>
+      </c>
+      <c r="AM8">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:39">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -1529,42 +1583,48 @@
         <v>50.00000000000001</v>
       </c>
       <c r="AC9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AD9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AE9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AH9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AI9">
         <v>285.6</v>
       </c>
       <c r="AJ9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AK9">
         <v>600</v>
       </c>
+      <c r="AL9">
+        <v>47.6</v>
+      </c>
+      <c r="AM9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:39">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -1642,42 +1702,48 @@
         <v>41.2</v>
       </c>
       <c r="AC10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AD10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AG10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AI10">
         <v>192.8</v>
       </c>
       <c r="AJ10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AK10">
         <v>600</v>
       </c>
+      <c r="AL10">
+        <v>32.13333333333333</v>
+      </c>
+      <c r="AM10">
+        <v>7</v>
+      </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:39">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -1755,42 +1821,48 @@
         <v>41.2</v>
       </c>
       <c r="AC11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AD11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AI11">
         <v>242.8</v>
       </c>
       <c r="AJ11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AK11">
         <v>600</v>
       </c>
+      <c r="AL11">
+        <v>40.46666666666667</v>
+      </c>
+      <c r="AM11">
+        <v>4</v>
+      </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:39">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -1868,42 +1940,48 @@
         <v>28.8</v>
       </c>
       <c r="AC12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AD12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AG12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AI12">
         <v>142</v>
       </c>
       <c r="AJ12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AK12">
         <v>600</v>
       </c>
+      <c r="AL12">
+        <v>23.66666666666667</v>
+      </c>
+      <c r="AM12">
+        <v>9</v>
+      </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:39">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -1981,31 +2059,37 @@
         <v>42</v>
       </c>
       <c r="AC13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AD13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AE13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AF13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AG13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AH13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AI13">
         <v>235.6</v>
       </c>
       <c r="AJ13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="AK13">
         <v>600</v>
+      </c>
+      <c r="AL13">
+        <v>39.26666666666667</v>
+      </c>
+      <c r="AM13">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>